<commit_message>
QA Test finish fix bug_UI7.1 fix bug_bugReport_UserInteract1
</commit_message>
<xml_diff>
--- a/QA/bugReport_TCD3.4.xlsx
+++ b/QA/bugReport_TCD3.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zork/Desktop/swift/StoreRoom/QA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D31846-BB52-C446-B88D-4F6C37B4A0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1EE061-6F9D-9746-B07F-E803D512DF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{7A968430-7FC1-B349-A0D4-34F5C039606C}"/>
   </bookViews>
@@ -256,39 +256,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -300,97 +280,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -417,18 +312,25 @@
     <dxf>
       <fill>
         <patternFill>
-          <fgColor theme="1"/>
-          <bgColor theme="6"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color theme="5" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -444,13 +346,17 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="5" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -765,7 +671,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -795,7 +701,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="2">
-        <v>45018</v>
+        <v>45017</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -931,42 +837,42 @@
       </c>
     </row>
     <row r="13" spans="1:6" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -978,34 +884,34 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B10">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="major">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="major">
       <formula>NOT(ISERROR(SEARCH("major",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="major">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="critical">
+      <formula>NOT(ISERROR(SEARCH("critical",B10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="major">
       <formula>NOT(ISERROR(SEARCH("major",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="minor">
-      <formula>NOT(ISERROR(SEARCH("minor",B10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="major">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="major">
       <formula>NOT(ISERROR(SEARCH("major",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="critical">
-      <formula>NOT(ISERROR(SEARCH("critical",B10)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="blocker">
+      <formula>NOT(ISERROR(SEARCH("blocker",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="blocker">
-      <formula>NOT(ISERROR(SEARCH("blocker",B10)))</formula>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="minor">
+      <formula>NOT(ISERROR(SEARCH("minor",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="низкий">
-      <formula>NOT(ISERROR(SEARCH("низкий",B11)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="высокий">
+      <formula>NOT(ISERROR(SEARCH("высокий",B11)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="средний">
       <formula>NOT(ISERROR(SEARCH("средний",B11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="высокий">
-      <formula>NOT(ISERROR(SEARCH("высокий",B11)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="низкий">
+      <formula>NOT(ISERROR(SEARCH("низкий",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>